<commit_message>
Update to Bakery Sales
Updating the sales file with more data to perform a activity.
</commit_message>
<xml_diff>
--- a/Course 2/Bakery Sales March 2020.xlsx
+++ b/Course 2/Bakery Sales March 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rittiv\Documents\GitHub\Google-Data-Analytics\Course 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9D7815-A43F-47BB-8C1D-0960B035656F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ABE6A9-B515-4B52-8E55-B2C502F520E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{ED27E09F-0831-49BA-939F-0726C5A5FBE7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -55,6 +52,24 @@
   </si>
   <si>
     <t>Pie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price </t>
+  </si>
+  <si>
+    <t>27/3</t>
+  </si>
+  <si>
+    <t>28/3</t>
+  </si>
+  <si>
+    <t>29/3</t>
+  </si>
+  <si>
+    <t>30/3</t>
+  </si>
+  <si>
+    <t>31/3</t>
   </si>
 </sst>
 </file>
@@ -64,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +91,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -427,113 +448,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C22D56-086E-4DF9-B3CC-1C595096DB2B}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="D3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" t="s">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4">
+      <c r="D13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" t="s">
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="D20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>